<commit_message>
add identified and not-identified ion intensity plot into the output file list for the html reports
</commit_message>
<xml_diff>
--- a/inst/extdata/report_output_files_description.xlsx
+++ b/inst/extdata/report_output_files_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanmichalik/Desktop/SpectR/single_module_R_scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanmichalik/Desktop/R_pipeline_analysis_scripts/SpectroPipeR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904EDD9F-6A6C-F843-AECF-A7AC7D5D6CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCD5FD5-2E40-224C-B257-DED3EB53FB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37640" yWindow="860" windowWidth="35540" windowHeight="16760" xr2:uid="{A1AC5CC0-2C2D-7043-AB91-EAF7258BCF92}"/>
+    <workbookView xWindow="15660" yWindow="860" windowWidth="35540" windowHeight="16760" xr2:uid="{A1AC5CC0-2C2D-7043-AB91-EAF7258BCF92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="179">
   <si>
     <t>Detected_ProteinGroups__stripped_peptide_count_per_condition_raw_data.csv</t>
   </si>
@@ -207,9 +206,6 @@
   </si>
   <si>
     <t>violin/boxplot of the normalization factors</t>
-  </si>
-  <si>
-    <t>violin/boxplot of the raw adn normalized intensities</t>
   </si>
   <si>
     <t>the hexbin plot shows the ion CV against the normalized ion intensity</t>
@@ -586,12 +582,21 @@
   <si>
     <t>simple cutoff test plot</t>
   </si>
+  <si>
+    <t>ion_intensity_Identified_notIdentified.png</t>
+  </si>
+  <si>
+    <t>violin/boxplot of the raw and normalized intensities</t>
+  </si>
+  <si>
+    <t>violin/boxplot of the ion intensites of identified and not-identified ions (not identified int.: imputed or background signal depending on the used Spectronaut settings)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1008,13 +1013,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2350DB-CEA1-604C-BA71-073458152755}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="17.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="75.83203125" style="2" customWidth="1"/>
@@ -1023,7 +1028,7 @@
     <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1037,7 +1042,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="36">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
@@ -1051,7 +1056,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="36">
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
@@ -1065,7 +1070,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="36">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -1079,7 +1084,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="36">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -1093,7 +1098,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="18">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -1107,7 +1112,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="18">
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
@@ -1121,7 +1126,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="18">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -1135,7 +1140,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="36">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -1149,7 +1154,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="18">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1163,7 +1168,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="18">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
@@ -1177,7 +1182,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="18">
       <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
@@ -1191,7 +1196,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="16">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
@@ -1202,10 +1207,10 @@
         <v>25</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16">
       <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
@@ -1216,10 +1221,10 @@
         <v>24</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16">
       <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
@@ -1230,10 +1235,10 @@
         <v>25</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16">
       <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
@@ -1244,10 +1249,10 @@
         <v>25</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18">
       <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
@@ -1261,7 +1266,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="18">
       <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
@@ -1275,7 +1280,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="18">
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
@@ -1289,7 +1294,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="18">
       <c r="A20" s="6" t="s">
         <v>19</v>
       </c>
@@ -1303,7 +1308,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="18">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
@@ -1317,7 +1322,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="18">
       <c r="A22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1331,7 +1336,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="54" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="54">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -1345,7 +1350,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="18">
       <c r="A24" s="6" t="s">
         <v>53</v>
       </c>
@@ -1356,10 +1361,10 @@
         <v>25</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18">
       <c r="A25" s="6" t="s">
         <v>53</v>
       </c>
@@ -1370,10 +1375,10 @@
         <v>25</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="36" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="36">
       <c r="A26" s="6" t="s">
         <v>53</v>
       </c>
@@ -1387,166 +1392,166 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="32">
       <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16">
       <c r="A28" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16">
       <c r="A29" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16">
+      <c r="A30" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="8" t="s">
+      <c r="C30" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+    <row r="31" spans="1:4" ht="16">
+      <c r="A31" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B30" s="6" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="16">
+      <c r="A32" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="8" t="s">
+      <c r="C32" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="6" t="s">
+    <row r="33" spans="1:4" ht="16">
+      <c r="A33" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="6" t="s">
+      <c r="C33" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="18">
+      <c r="A34" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="C34" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="18">
       <c r="A35" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16">
+      <c r="A36" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16">
+      <c r="A37" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="8" t="s">
+      <c r="C37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" s="6" t="s">
+    <row r="38" spans="1:4" ht="16">
+      <c r="A38" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>25</v>
@@ -1555,306 +1560,306 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="16">
       <c r="A39" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16">
+      <c r="A40" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="16">
+      <c r="A41" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D39" s="8" t="s">
+      <c r="C41" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="6" t="s">
+    <row r="42" spans="1:4" ht="16">
+      <c r="A42" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="8" t="s">
+      <c r="C42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="6" t="s">
+    <row r="43" spans="1:4" ht="16">
+      <c r="A43" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="8" t="s">
+      <c r="C43" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" s="6" t="s">
+    <row r="44" spans="1:4" ht="32">
+      <c r="A44" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="C44" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="6" t="s">
+    <row r="45" spans="1:4" ht="16">
+      <c r="A45" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43" s="8" t="s">
+      <c r="C45" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="6" t="s">
+    <row r="46" spans="1:4" ht="16">
+      <c r="A46" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="8" t="s">
+      <c r="C46" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" s="6" t="s">
+    <row r="47" spans="1:4" ht="16">
+      <c r="A47" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D45" s="8" t="s">
+      <c r="C47" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D46" s="8" t="s">
+    <row r="48" spans="1:4" ht="16">
+      <c r="A48" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+      <c r="C48" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B47" s="6" t="s">
+    </row>
+    <row r="49" spans="1:4" ht="16">
+      <c r="A49" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D47" s="8" t="s">
+      <c r="C49" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B48" s="6" t="s">
+    <row r="50" spans="1:4" ht="16">
+      <c r="A50" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="8" t="s">
+      <c r="C50" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B49" s="6" t="s">
+    <row r="51" spans="1:4" ht="16">
+      <c r="A51" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="16">
+      <c r="A52" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="16">
+      <c r="A53" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="16">
+      <c r="A54" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="16">
+      <c r="A55" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="16">
+      <c r="A56" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D54" s="8" t="s">
+      <c r="C56" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B55" s="6" t="s">
+    <row r="57" spans="1:4" ht="16">
+      <c r="A57" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C55" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D55" s="8" t="s">
+      <c r="C57" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" s="8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B56" s="6" t="s">
+    <row r="58" spans="1:4" ht="16">
+      <c r="A58" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D56" s="8" t="s">
+      <c r="C58" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B57" s="6" t="s">
+    <row r="59" spans="1:4" ht="16">
+      <c r="A59" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B58" s="6" t="s">
+      <c r="C59" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="32">
+      <c r="A60" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>25</v>
@@ -1863,340 +1868,354 @@
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="32">
       <c r="A61" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="32">
+      <c r="A62" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="32">
+      <c r="A63" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C61" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D61" s="8" t="s">
+      <c r="C63" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" s="10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B62" s="6" t="s">
+    <row r="64" spans="1:4" ht="32">
+      <c r="A64" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C62" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D62" s="10" t="s">
+      <c r="C64" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" s="10" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B63" s="6" t="s">
+    <row r="65" spans="1:4" ht="16">
+      <c r="A65" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C63" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D63" s="10" t="s">
+      <c r="C65" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B64" s="6" t="s">
+    <row r="66" spans="1:4" ht="16">
+      <c r="A66" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C64" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D64" s="8" t="s">
+      <c r="C66" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B65" s="6" t="s">
+    <row r="67" spans="1:4" ht="16">
+      <c r="A67" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B67" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C65" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D65" s="8" t="s">
+      <c r="C67" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67" s="8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B66" s="6" t="s">
+    <row r="68" spans="1:4" ht="16">
+      <c r="A68" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="16">
+      <c r="A69" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C66" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D66" s="8" t="s">
+      <c r="C69" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D69" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B68" s="6" t="s">
+    <row r="70" spans="1:4" ht="16">
+      <c r="A70" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C68" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D68" s="8" t="s">
+      <c r="C70" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="16">
+      <c r="A71" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B70" s="6" t="s">
+      <c r="C71" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="32">
+      <c r="A72" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B71" s="6" t="s">
+      <c r="C72" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="16">
+      <c r="A73" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C71" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>149</v>
-      </c>
       <c r="C73" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="16">
       <c r="A74" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="16">
+      <c r="A75" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="16">
+      <c r="A76" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="16">
+      <c r="A77" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="16">
+      <c r="A78" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="16">
+      <c r="A79" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="25">
+      <c r="A80" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="32">
+      <c r="A81" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="32">
+      <c r="A82" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D82" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B74" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="25" x14ac:dyDescent="0.35">
-      <c r="A79" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D80" s="8" t="s">
+    </row>
+    <row r="83" spans="1:4" ht="32">
+      <c r="A83" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D83" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A82" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B82" s="6" t="s">
+    <row r="84" spans="1:4" ht="32">
+      <c r="A84" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A83" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A84" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="32">
+      <c r="A85" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>